<commit_message>
adding to central repo
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -556,12 +556,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>